<commit_message>
small refactoring: move some logic from motors to speedctrl file; move pin initializations from main file to motors and sensors files
</commit_message>
<xml_diff>
--- a/sensors-data/sensorsData.xlsx
+++ b/sensors-data/sensorsData.xlsx
@@ -8,25 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkhalzov/Documents/PlatformIO/Projects/190602-140824-uno/sensors-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BECE13-E867-474C-9A6A-0D4EA5AC2441}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24BDE9F-8D72-DE40-9E4D-B9F8D6891ECA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensorsData" sheetId="1" r:id="rId1"/>
     <sheet name="sensorsData (2)" sheetId="2" r:id="rId2"/>
     <sheet name="SensorsData (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="SensorsData (4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'SensorsData (3)'!$A$1:$A$112</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'SensorsData (3)'!$B$1:$B$112</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'SensorsData (3)'!$C$1:$C$112</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'SensorsData (3)'!$D$1:$D$112</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'SensorsData (3)'!$A$1:$A$112</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'SensorsData (3)'!$B$1:$B$112</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'SensorsData (3)'!$C$1:$C$112</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'SensorsData (3)'!$D$1:$D$112</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6460,6 +6451,1183 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.056250736206881E-2"/>
+          <c:y val="6.3534731425898494E-2"/>
+          <c:w val="0.95451673115083857"/>
+          <c:h val="0.83535588991970067"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'SensorsData (4)'!$A$1:$A$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0FA1-9345-A8C5-77918529EC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'SensorsData (4)'!$B$1:$B$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0FA1-9345-A8C5-77918529EC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'SensorsData (4)'!$C$1:$C$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0FA1-9345-A8C5-77918529EC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'SensorsData (4)'!$D$1:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0FA1-9345-A8C5-77918529EC01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="938061087"/>
+        <c:axId val="1049875951"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="938061087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1049875951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1049875951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="938061087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6660,6 +7828,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -8725,6 +9933,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9405,15 +11129,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9421,6 +11145,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297096DE-EBAF-884B-A006-40C1AEC8FF90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EB4C4B-85B1-CB49-8538-760A773068B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11653,8 +13418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DFE6C5-21DC-554A-A6DE-D93AA163FD8B}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13231,4 +14996,944 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CB9DBC-AA9D-8F40-AD8C-A33B4B7BE05F}">
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>84</v>
+      </c>
+      <c r="B1">
+        <v>74</v>
+      </c>
+      <c r="C1">
+        <v>66</v>
+      </c>
+      <c r="D1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>109</v>
+      </c>
+      <c r="C2">
+        <v>105</v>
+      </c>
+      <c r="D2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>128</v>
+      </c>
+      <c r="B4">
+        <v>129</v>
+      </c>
+      <c r="C4">
+        <v>128</v>
+      </c>
+      <c r="D4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>135</v>
+      </c>
+      <c r="B5">
+        <v>133</v>
+      </c>
+      <c r="C5">
+        <v>133</v>
+      </c>
+      <c r="D5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>139</v>
+      </c>
+      <c r="B6">
+        <v>141</v>
+      </c>
+      <c r="C6">
+        <v>138</v>
+      </c>
+      <c r="D6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>143</v>
+      </c>
+      <c r="B7">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>148</v>
+      </c>
+      <c r="D7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>148</v>
+      </c>
+      <c r="B8">
+        <v>154</v>
+      </c>
+      <c r="C8">
+        <v>152</v>
+      </c>
+      <c r="D8">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>149</v>
+      </c>
+      <c r="B9">
+        <v>159</v>
+      </c>
+      <c r="C9">
+        <v>152</v>
+      </c>
+      <c r="D9">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>148</v>
+      </c>
+      <c r="B10">
+        <v>159</v>
+      </c>
+      <c r="C10">
+        <v>153</v>
+      </c>
+      <c r="D10">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>148</v>
+      </c>
+      <c r="B11">
+        <v>159</v>
+      </c>
+      <c r="C11">
+        <v>152</v>
+      </c>
+      <c r="D11">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>149</v>
+      </c>
+      <c r="B12">
+        <v>146</v>
+      </c>
+      <c r="C12">
+        <v>153</v>
+      </c>
+      <c r="D12">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>145</v>
+      </c>
+      <c r="B13">
+        <v>139</v>
+      </c>
+      <c r="C13">
+        <v>144</v>
+      </c>
+      <c r="D13">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>141</v>
+      </c>
+      <c r="B14">
+        <v>135</v>
+      </c>
+      <c r="C14">
+        <v>139</v>
+      </c>
+      <c r="D14">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>137</v>
+      </c>
+      <c r="B15">
+        <v>130</v>
+      </c>
+      <c r="C15">
+        <v>134</v>
+      </c>
+      <c r="D15">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>132</v>
+      </c>
+      <c r="B16">
+        <v>123</v>
+      </c>
+      <c r="C16">
+        <v>127</v>
+      </c>
+      <c r="D16">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>124</v>
+      </c>
+      <c r="B17">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>118</v>
+      </c>
+      <c r="D17">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>110</v>
+      </c>
+      <c r="B18">
+        <v>107</v>
+      </c>
+      <c r="C18">
+        <v>110</v>
+      </c>
+      <c r="D18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>99</v>
+      </c>
+      <c r="B19">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <v>97</v>
+      </c>
+      <c r="D19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>96</v>
+      </c>
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <v>91</v>
+      </c>
+      <c r="D20">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>90</v>
+      </c>
+      <c r="C21">
+        <v>92</v>
+      </c>
+      <c r="D21">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>96</v>
+      </c>
+      <c r="B22">
+        <v>90</v>
+      </c>
+      <c r="C22">
+        <v>93</v>
+      </c>
+      <c r="D22">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <v>111</v>
+      </c>
+      <c r="C23">
+        <v>104</v>
+      </c>
+      <c r="D23">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>115</v>
+      </c>
+      <c r="B24">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>115</v>
+      </c>
+      <c r="D24">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>125</v>
+      </c>
+      <c r="B25">
+        <v>125</v>
+      </c>
+      <c r="C25">
+        <v>125</v>
+      </c>
+      <c r="D25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>130</v>
+      </c>
+      <c r="B26">
+        <v>130</v>
+      </c>
+      <c r="C26">
+        <v>131</v>
+      </c>
+      <c r="D26">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>135</v>
+      </c>
+      <c r="B27">
+        <v>136</v>
+      </c>
+      <c r="C27">
+        <v>134</v>
+      </c>
+      <c r="D27">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>141</v>
+      </c>
+      <c r="B28">
+        <v>142</v>
+      </c>
+      <c r="C28">
+        <v>143</v>
+      </c>
+      <c r="D28">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>144</v>
+      </c>
+      <c r="B29">
+        <v>147</v>
+      </c>
+      <c r="C29">
+        <v>149</v>
+      </c>
+      <c r="D29">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>148</v>
+      </c>
+      <c r="B30">
+        <v>155</v>
+      </c>
+      <c r="C30">
+        <v>155</v>
+      </c>
+      <c r="D30">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>150</v>
+      </c>
+      <c r="B31">
+        <v>159</v>
+      </c>
+      <c r="C31">
+        <v>155</v>
+      </c>
+      <c r="D31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>150</v>
+      </c>
+      <c r="B32">
+        <v>160</v>
+      </c>
+      <c r="C32">
+        <v>154</v>
+      </c>
+      <c r="D32">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>151</v>
+      </c>
+      <c r="B33">
+        <v>160</v>
+      </c>
+      <c r="C33">
+        <v>155</v>
+      </c>
+      <c r="D33">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>149</v>
+      </c>
+      <c r="B34">
+        <v>146</v>
+      </c>
+      <c r="C34">
+        <v>153</v>
+      </c>
+      <c r="D34">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>147</v>
+      </c>
+      <c r="B35">
+        <v>140</v>
+      </c>
+      <c r="C35">
+        <v>144</v>
+      </c>
+      <c r="D35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>143</v>
+      </c>
+      <c r="B36">
+        <v>135</v>
+      </c>
+      <c r="C36">
+        <v>139</v>
+      </c>
+      <c r="D36">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>137</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+      <c r="C37">
+        <v>133</v>
+      </c>
+      <c r="D37">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>129</v>
+      </c>
+      <c r="B38">
+        <v>122</v>
+      </c>
+      <c r="C38">
+        <v>128</v>
+      </c>
+      <c r="D38">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>121</v>
+      </c>
+      <c r="B39">
+        <v>117</v>
+      </c>
+      <c r="C39">
+        <v>118</v>
+      </c>
+      <c r="D39">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>111</v>
+      </c>
+      <c r="B40">
+        <v>105</v>
+      </c>
+      <c r="C40">
+        <v>107</v>
+      </c>
+      <c r="D40">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>99</v>
+      </c>
+      <c r="B41">
+        <v>92</v>
+      </c>
+      <c r="C41">
+        <v>93</v>
+      </c>
+      <c r="D41">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>98</v>
+      </c>
+      <c r="B42">
+        <v>92</v>
+      </c>
+      <c r="C42">
+        <v>87</v>
+      </c>
+      <c r="D42">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>97</v>
+      </c>
+      <c r="B43">
+        <v>92</v>
+      </c>
+      <c r="C43">
+        <v>87</v>
+      </c>
+      <c r="D43">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>97</v>
+      </c>
+      <c r="B44">
+        <v>91</v>
+      </c>
+      <c r="C44">
+        <v>86</v>
+      </c>
+      <c r="D44">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>99</v>
+      </c>
+      <c r="B45">
+        <v>103</v>
+      </c>
+      <c r="C45">
+        <v>115</v>
+      </c>
+      <c r="D45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>115</v>
+      </c>
+      <c r="B46">
+        <v>117</v>
+      </c>
+      <c r="C46">
+        <v>122</v>
+      </c>
+      <c r="D46">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>125</v>
+      </c>
+      <c r="B47">
+        <v>127</v>
+      </c>
+      <c r="C47">
+        <v>126</v>
+      </c>
+      <c r="D47">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>133</v>
+      </c>
+      <c r="B48">
+        <v>134</v>
+      </c>
+      <c r="C48">
+        <v>131</v>
+      </c>
+      <c r="D48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>137</v>
+      </c>
+      <c r="B49">
+        <v>136</v>
+      </c>
+      <c r="C49">
+        <v>133</v>
+      </c>
+      <c r="D49">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>143</v>
+      </c>
+      <c r="B50">
+        <v>144</v>
+      </c>
+      <c r="C50">
+        <v>142</v>
+      </c>
+      <c r="D50">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>147</v>
+      </c>
+      <c r="B51">
+        <v>149</v>
+      </c>
+      <c r="C51">
+        <v>148</v>
+      </c>
+      <c r="D51">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>150</v>
+      </c>
+      <c r="B52">
+        <v>157</v>
+      </c>
+      <c r="C52">
+        <v>155</v>
+      </c>
+      <c r="D52">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>155</v>
+      </c>
+      <c r="B53">
+        <v>162</v>
+      </c>
+      <c r="C53">
+        <v>154</v>
+      </c>
+      <c r="D53">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>154</v>
+      </c>
+      <c r="B54">
+        <v>161</v>
+      </c>
+      <c r="C54">
+        <v>155</v>
+      </c>
+      <c r="D54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>155</v>
+      </c>
+      <c r="B55">
+        <v>162</v>
+      </c>
+      <c r="C55">
+        <v>155</v>
+      </c>
+      <c r="D55">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>151</v>
+      </c>
+      <c r="B56">
+        <v>147</v>
+      </c>
+      <c r="C56">
+        <v>155</v>
+      </c>
+      <c r="D56">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>149</v>
+      </c>
+      <c r="B57">
+        <v>142</v>
+      </c>
+      <c r="C57">
+        <v>146</v>
+      </c>
+      <c r="D57">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>144</v>
+      </c>
+      <c r="B58">
+        <v>136</v>
+      </c>
+      <c r="C58">
+        <v>140</v>
+      </c>
+      <c r="D58">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>140</v>
+      </c>
+      <c r="B59">
+        <v>133</v>
+      </c>
+      <c r="C59">
+        <v>136</v>
+      </c>
+      <c r="D59">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>132</v>
+      </c>
+      <c r="B60">
+        <v>124</v>
+      </c>
+      <c r="C60">
+        <v>132</v>
+      </c>
+      <c r="D60">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>124</v>
+      </c>
+      <c r="B61">
+        <v>117</v>
+      </c>
+      <c r="C61">
+        <v>122</v>
+      </c>
+      <c r="D61">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>113</v>
+      </c>
+      <c r="B62">
+        <v>110</v>
+      </c>
+      <c r="C62">
+        <v>112</v>
+      </c>
+      <c r="D62">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>100</v>
+      </c>
+      <c r="B63">
+        <v>96</v>
+      </c>
+      <c r="C63">
+        <v>99</v>
+      </c>
+      <c r="D63">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>99</v>
+      </c>
+      <c r="B64">
+        <v>93</v>
+      </c>
+      <c r="C64">
+        <v>93</v>
+      </c>
+      <c r="D64">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>97</v>
+      </c>
+      <c r="B65">
+        <v>92</v>
+      </c>
+      <c r="C65">
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>98</v>
+      </c>
+      <c r="B66">
+        <v>93</v>
+      </c>
+      <c r="C66">
+        <v>92</v>
+      </c>
+      <c r="D66">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>